<commit_message>
Re-added files without token
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="168">
-  <si>
-    <t>ЧИСЕЛЬНИК</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
+  <si>
+    <t>ЗНАМЕННИК</t>
   </si>
   <si>
     <t>Ф 1/1</t>
@@ -67,6 +67,52 @@
   </si>
   <si>
     <t>Е1/2</t>
+  </si>
+  <si>
+    <t>Інформатика
+Мигович С.М.
+гнк 303</t>
+  </si>
+  <si>
+    <t>Історія: Україна і світ
+Кириленко А.О.
+гнк 118</t>
+  </si>
+  <si>
+    <t>Інформатика
+Римар Р.В.
+гнк 320</t>
+  </si>
+  <si>
+    <t>Природничі науки (Фізика. астрономія)
+Василенко О.М.
+гнк 319</t>
+  </si>
+  <si>
+    <t>Природничі науки (Хімія)
+Бабич О.А.
+карп 202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Українська література
+Бугайова А.С.
+гнк 313
+</t>
+  </si>
+  <si>
+    <t>Іноземна мова
+Коновалова Т.В.
+гнк 02</t>
+  </si>
+  <si>
+    <t>Природничі науки (Географія)
+Савенко Л.М.
+гнк 319</t>
+  </si>
+  <si>
+    <t>Українська мова
+Гордієць І.А.
+гнк 103</t>
   </si>
   <si>
     <t>Зарубіжна література
@@ -74,149 +120,109 @@
 гнк 118</t>
   </si>
   <si>
+    <t>Природничі науки (Біологія, основи
+екології, екологічна етика)
+Кругленко А.М.
+карп 304</t>
+  </si>
+  <si>
+    <t>Українська література
+Марценюк А.В.
+гнк 217</t>
+  </si>
+  <si>
+    <t>Українська мова
+Мусініна К.М.
+гнк 102</t>
+  </si>
+  <si>
+    <t>Зарубіжна література
+Павленко Т.В.
+гнк 320</t>
+  </si>
+  <si>
+    <t>Природничі науки (Географія)
+Савенко Л.М.
+гнк 117</t>
+  </si>
+  <si>
+    <t>Інформатика
+Римар Р.В.
+гнк 303</t>
+  </si>
+  <si>
     <t>Іноземна мова
 Сушко Н.М.
-гнк 02</t>
+бібліотека гуртожитк</t>
+  </si>
+  <si>
+    <t>Інформатика
+Бєлова С.А.
+гнк 316</t>
+  </si>
+  <si>
+    <t>Українська література 
+Бугайова А.С.
+гнк 319</t>
+  </si>
+  <si>
+    <t>Природничі науки (Географія)
+Савенко Л.М.
+гнк 313</t>
+  </si>
+  <si>
+    <t>Математика (алгебра і
+початки аналізу та геометрія)
+Сігачова Н.П.
+гнк 320</t>
+  </si>
+  <si>
+    <t>Інформатика
+Римар Р.В.
+гнк 220</t>
+  </si>
+  <si>
+    <t>Зарубіжна література
+Павленко Т.В.
+карп</t>
   </si>
   <si>
     <t>Природничі науки (Біологія,
 основи екології, кологічна етика)
 Кругленко А.М.
-карп 205</t>
-  </si>
-  <si>
-    <t>Українська література
-Марценюк А.В.
-гнк 102</t>
+гнк 113</t>
+  </si>
+  <si>
+    <t>Математика (алгебра і
+початки аналізу та геометрія)
+Красовський О.О.
+гнк 117</t>
+  </si>
+  <si>
+    <t>Фізична культура
+Рябов Є.І.
+ПК</t>
   </si>
   <si>
     <t>Історія: Україна і світ
 Кириленко А.О.
-карп</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і
-початки аналізу та геометрія)
-Сігачова Н.П.
 гнк 111</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
-Гузенко Ю.І.
-гнк 304</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і
-початки аналізу та геометрія)
-Пєткова О.В.
-гнк 117</t>
-  </si>
-  <si>
-    <t>Українська мова
-Бугайова А.С.
-карп/м</t>
-  </si>
-  <si>
-    <t>Зарубіжна література
-Павленко Т.В.
-гнк 101</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і 
-початки аналізу та геометрія)
-Сігачова Н.П.
-гнк 118</t>
-  </si>
-  <si>
-    <t>Українська література
-Марценюк А.В.
-гнк 217</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
-Кириленко А.О.
-карп 212</t>
-  </si>
-  <si>
-    <t>Зарубіжна література
-Павленко Т.В.
-карп 223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Математика (алгебра і
-початки аналізу та геометрія)
-Пєткова О.В.
-</t>
-  </si>
-  <si>
-    <t>Природничі науки (Біологія, основи
-екології, екологічна етика)
-Кругленко А.М.
-карп 202</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
-Гузенко Ю.І.
-бібліотека гуртожитку</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
-Кириленко А.О.
-карп 223</t>
   </si>
   <si>
     <t>Природничі науки (Фізика. астрономія)
 Василенко О.М.
-гнк 103</t>
-  </si>
-  <si>
-    <t>Іноземна мова
-Коновалова Т.В.
-гнк 02</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і
-початки аналізу та геометрія)
-Рура Г.В.
-гнк 320</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і
-початки аналізу та геометрія)
-Сігачова Н.П.
-гнк 112</t>
-  </si>
-  <si>
-    <t>Математика (алгебра і
-початки аналізу та геометрія)
-Пєткова О.В.
-гнк 101</t>
+гнк 223</t>
+  </si>
+  <si>
+    <t>Пиродничі науки (Хімія)
+Бабич О.А.
+гнк 212</t>
   </si>
   <si>
     <t>Природничі науки (Біологія,
 основи екології, кологічна етика)
 Кругленко А.М.
-карп 404</t>
-  </si>
-  <si>
-    <t>Українська мова
-Мусініна К.М.
-гнк 102</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
-Гузенко Ю.І
-гнк 223</t>
-  </si>
-  <si>
-    <t>Українська мова
-Гордієць І.А.
-гнк 212</t>
-  </si>
-  <si>
-    <t>Українська література
-Бугайова А.С.
-гнк 211</t>
+гнк 213</t>
   </si>
   <si>
     <t>Ф 2/1</t>
@@ -273,130 +279,155 @@
     <t>Аі 2/2</t>
   </si>
   <si>
-    <t>Бухгалтерський облік
-Марковська Т.С
-гнк 111</t>
-  </si>
-  <si>
-    <t>Технології
-Манушкіна Т. М
-карп 407</t>
+    <t>Фінанси підприємства
+Киричук О. М
+гнк 316</t>
+  </si>
+  <si>
+    <t>Іноземна мова
+Коновалова Т.В
+гнк 02</t>
+  </si>
+  <si>
+    <t>Основи філософських знань
+Гузенко Ю.І.
+гнк 324</t>
+  </si>
+  <si>
+    <t>Фізіологія рослин з основами мікробіології
+Кругленко А. М
+карп 114</t>
   </si>
   <si>
     <t>Математика (алгебра, початки аналізу та геометрія)
 Рура А. В
-м 201</t>
-  </si>
-  <si>
-    <t>Історія: Україна і світ
+гнк 324</t>
+  </si>
+  <si>
+    <t>Історія: Уккраїна і світ
 Кириленко А. О
-гнк 112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Основи філософських знань
-Рачков О.М
-карп </t>
+гнк 111</t>
+  </si>
+  <si>
+    <t>Фізичне виховання
+Рябов Є. І
+карп с/з</t>
   </si>
   <si>
     <t>Технології
+Потапова О. А
+гнк 100</t>
+  </si>
+  <si>
+    <t>Фізика
+Василенко О. М
+гнк 117</t>
+  </si>
+  <si>
+    <t>Технології
+Римар Р.В.
+гнк 303.</t>
+  </si>
+  <si>
+    <t>Біологія (біологія рослин, бтаніка)
+Стебліченко О. І
+гнк 316</t>
+  </si>
+  <si>
+    <t>Математика (алгебра, початки аналізу та геометрія)
+Рура А. В
+гнк 101</t>
+  </si>
+  <si>
+    <t>Основи філософських знань. Політологія. Соціологія
+Гузенко Ю.І
+гнк 320</t>
+  </si>
+  <si>
+    <t>Українська мова
+Бугайова А.С.
+гнк 103</t>
+  </si>
+  <si>
+    <t>Фінанси підприємства
 Киричук О. М
-гнк 212</t>
+гнк 116</t>
+  </si>
+  <si>
+    <t>Математика (алгебра, початки аналізу та геометрія)
+Сігачова Н. П
+гнк 324</t>
   </si>
   <si>
     <t>Економічна теорія
 Мандрик Л. П
-гнк 220</t>
-  </si>
-  <si>
-    <t>Українська мова
-Гордієь І. А
-гнк 02</t>
-  </si>
-  <si>
-    <t>Українська мова
-Мусініна К. М
-гнк 103</t>
+гнк 212</t>
   </si>
   <si>
     <t>Математика (алгебра, початки аналізу та геометрія)
-Рура А. В
-м 208</t>
-  </si>
-  <si>
-    <t>Іноземна мова
-Сушко Н. М
-м 211</t>
-  </si>
-  <si>
-    <t>Фізичне виховання
-Рябов Є. І
-гнк с/з</t>
-  </si>
-  <si>
-    <t>Іноземна мова
-Коновалова Т. В
-м 206</t>
-  </si>
-  <si>
-    <t>Українська мова
-Гордієць І. А
-гнк 103</t>
-  </si>
-  <si>
-    <t>Економічна теорія
-Мандрик Л. П
-гнк 320</t>
-  </si>
-  <si>
-    <t>Іноземна мова
-Сушко Н. М
-гнк 313</t>
-  </si>
-  <si>
-    <t>Біологія (біологія рослин, бтаніка)
-Стебліченко О. І
+Пєткова О. В
 гнк 211</t>
+  </si>
+  <si>
+    <t>Історія:Україна і світ
+Кириленко А. О
+карп</t>
   </si>
   <si>
     <t>Основи філософських знань
 Рачков О.М
-карп 112</t>
-  </si>
-  <si>
-    <t>Математика (алгебра, початки аналізу та геометрія)
-Рура А. В
-м 203</t>
+карп</t>
+  </si>
+  <si>
+    <t>Хімія (неорганічна хімія)
+Кругленко А. М
+м 213</t>
+  </si>
+  <si>
+    <t>Підприємницька діяльність
+Кошміла В. В
+м 303</t>
   </si>
   <si>
     <t>Фізика (Теоретичні основи електротехніки,
 інженерна механіка)
 Василенко О.М.
-гнк 111</t>
-  </si>
-  <si>
-    <t>Українська мова
-Бугайова А.С.
-карп 206</t>
-  </si>
-  <si>
-    <t>Бухгалтерський облік
-Марковська Т.С
+гнк 118</t>
+  </si>
+  <si>
+    <t>Математика (алгебра, початки анлізу та геометрія)
+Рура Г.В.
+гнк101</t>
+  </si>
+  <si>
+    <t>Іноземна мова
+Коновалова Т. В
+гнк 02</t>
+  </si>
+  <si>
+    <t>Політична економія
+Мандрик Л. П
 гнк 319</t>
   </si>
   <si>
-    <t>Статистика
-Іваненко Т.Я.
-м 213</t>
-  </si>
-  <si>
-    <t>Українська мова
-Гордієць І. А
-гнк 211</t>
-  </si>
-  <si>
-    <t>Основи генетики та селекції с/г тварин
-Гиль М.І.
-карп 202</t>
+    <t>Фізика
+Василенко О. М
+гнк 324</t>
+  </si>
+  <si>
+    <t>Біологія (біологія рослин, бтаніка)
+Стебліченко О. І
+гнк 313</t>
+  </si>
+  <si>
+    <t>Технології
+Данильчук Г. А
+карп 223</t>
+  </si>
+  <si>
+    <t>Підприємницька діяльність
+Кошміла В.В
+м 103</t>
   </si>
   <si>
     <t>Українська мова
@@ -404,180 +435,191 @@
 гнк 102</t>
   </si>
   <si>
-    <t>Основи філософських знань
-Рачков О.М
-карп 410</t>
+    <t>Математика (алгебра, початки анлізу та геометрія)
+Рура Г.В.
+гнк 101</t>
+  </si>
+  <si>
+    <t>Іноземна мова
+Сушко Н.М.
+бібліотека гуртожитку</t>
+  </si>
+  <si>
+    <t>Історія: Україна і світ
+Яворська І. В
+гнк 118</t>
   </si>
   <si>
     <t>Математика (алгебра, початки аналізу та геометрія)
-Сігачова Н. П
-гнк 213</t>
-  </si>
-  <si>
-    <t>Бухгалтерський облік
+Рура А. В
+гнк 117</t>
+  </si>
+  <si>
+    <t>Основи теплотехніки і гідравліки
+ Павленко О.В.
+крил 109</t>
+  </si>
+  <si>
+    <t>Ф 3/1</t>
+  </si>
+  <si>
+    <t>Б 3/1</t>
+  </si>
+  <si>
+    <t>П 3/1</t>
+  </si>
+  <si>
+    <t>Г 3/1</t>
+  </si>
+  <si>
+    <t>Г 3/2</t>
+  </si>
+  <si>
+    <t>М 3/1</t>
+  </si>
+  <si>
+    <t>М 3/2</t>
+  </si>
+  <si>
+    <t>Р 3/1</t>
+  </si>
+  <si>
+    <t>Р 3/2</t>
+  </si>
+  <si>
+    <t>Т 3/1</t>
+  </si>
+  <si>
+    <t>Е 3/1</t>
+  </si>
+  <si>
+    <t>Аі 3/1</t>
+  </si>
+  <si>
+    <t>Підприємницька діяльність. Планування і організація діяльності аграрних формувань
+Кошміла В.В
+м 201</t>
+  </si>
+  <si>
+    <t>Основиохорони праці. Охорона праці і галузі. БЖД. Основи екології
+Рачков О. М
+гнк 319</t>
+  </si>
+  <si>
+    <t>ЗНАЧЕННЯ КОЛЬОРІВ</t>
+  </si>
+  <si>
+    <t>Підприємницька діяльність. Планування і організація діяльності аграрних формувань
+Кошміла В.В 
+м 208</t>
+  </si>
+  <si>
+    <t>Контроль і ревізія
+Киричук О. М
+гнк 113</t>
+  </si>
+  <si>
+    <t>Бухгалтерський облік. Фінансовий облік
 Марковська Т. С
-гнк 316</t>
-  </si>
-  <si>
-    <t>Фінанси підприємства
-Киричук О. М
-гнк 223</t>
+гнк 116</t>
+  </si>
+  <si>
+    <t>Захист рослин
+Бабич О. А
+карп 216</t>
+  </si>
+  <si>
+    <t>Прикладна математика
+Красовський О. О
+карп 107</t>
+  </si>
+  <si>
+    <t>- змінилась/ відмінилась/доставилась пара</t>
+  </si>
+  <si>
+    <t>Облік і аналіз ЗЕД
+Марковська Т.С
+гнк 309</t>
+  </si>
+  <si>
+    <t>Продовольче товарознавство
+Потапова О. А
+гнк 100</t>
+  </si>
+  <si>
+    <t>Технології зберігання іпереробки с/г продукції
+Стебліченко О. І
+гнк 111</t>
+  </si>
+  <si>
+    <t>Захист рослин
+Бабич О. А
+карп 223</t>
+  </si>
+  <si>
+    <t>Тратори і автомобілі
+Павленко
+крил 014</t>
+  </si>
+  <si>
+    <t>- змінилась аудиторія</t>
+  </si>
+  <si>
+    <t>Управлінський облік
+Марковська Т.С
+гнк116</t>
+  </si>
+  <si>
+    <t>Інфораційні системи і технології в комерційних банках
+Мигович С. М
+гнк 305</t>
+  </si>
+  <si>
+    <t>Організація і технологія обслуговування в закладах готельного господарства
+Тишкевич В.В.
+м 108</t>
+  </si>
+  <si>
+    <t>Комерційне право
+Сідлецька Л. Л
+гнк 217</t>
   </si>
   <si>
     <t>Фізичне виховання
 Рябов Є. І</t>
   </si>
   <si>
-    <t>Фізична культура
-Коржевський М. Ю</t>
-  </si>
-  <si>
-    <t>Інформаційні системи в готельно-ресторанному господарстві
-Мигович С. М
-гнк 305</t>
-  </si>
-  <si>
-    <t>Ф 3/1</t>
-  </si>
-  <si>
-    <t>Б 3/1</t>
-  </si>
-  <si>
-    <t>П 3/1</t>
-  </si>
-  <si>
-    <t>Г 3/1</t>
-  </si>
-  <si>
-    <t>Г 3/2</t>
-  </si>
-  <si>
-    <t>М 3/1</t>
-  </si>
-  <si>
-    <t>М 3/2</t>
-  </si>
-  <si>
-    <t>Р 3/1</t>
-  </si>
-  <si>
-    <t>Р 3/2</t>
-  </si>
-  <si>
-    <t>Т 3/1</t>
-  </si>
-  <si>
-    <t>Е 3/1</t>
-  </si>
-  <si>
-    <t>Аі 3/1</t>
-  </si>
-  <si>
-    <t>Технології зберігання іпереробки с/г продукції
-Стебліченко О. І
-гнк 212</t>
-  </si>
-  <si>
-    <t>Механізація і автоматизація с/г виробництва
-Корж Д. В
-карп 219</t>
-  </si>
-  <si>
-    <t>Тратори і автомобілі
-Павленко О.В
-карп 304</t>
-  </si>
-  <si>
-    <t>ЗНАЧЕННЯ КОЛЬОРІВ</t>
-  </si>
-  <si>
-    <t>Управлінський облік
-Марковська Т. С
-м 209</t>
-  </si>
-  <si>
-    <t>Комерційна діяльність
-Потапова О. А
-гнк 100</t>
-  </si>
-  <si>
-    <t>Трудове право
-Кисляк Г. М
-гнк 303</t>
-  </si>
-  <si>
-    <t>Інформатика і компьютерна техніка
-Мигович С. М
-гнк 111</t>
-  </si>
-  <si>
-    <t>Механізація і автоматизація с/г виробництва
-Корж Д. В
-карп 222</t>
-  </si>
-  <si>
-    <t>Гідропривід с/г техніки
-Павленко О.В
-карп 304</t>
-  </si>
-  <si>
-    <t>- змінилась/ відмінилась/доставилась пара</t>
-  </si>
-  <si>
-    <t>Фінанси. Гроші та кредит
-Киричук О. М
-гнк 310</t>
-  </si>
-  <si>
-    <t>Інформатика і компьютерна техніка
-Мигович С. М
-гнк 305</t>
-  </si>
-  <si>
-    <t>Дослідження операцій. Економетрія
-Красовський О. О
-гнк 304</t>
-  </si>
-  <si>
-    <t>Фізична культура
-Фаріонов В.М.
-гнк с/з</t>
-  </si>
-  <si>
-    <t>- змінилась аудиторія</t>
-  </si>
-  <si>
-    <t>Контроль і ревізія
-Киричук О. М
-гнк 116</t>
-  </si>
-  <si>
-    <t>Ціноутворення
-Прогонюк Л.Ю
-м 103</t>
-  </si>
-  <si>
-    <t>Товарознавство продукції твариннцитва
-Потапова О. А
-гнк 100</t>
-  </si>
-  <si>
-    <t>Прикладна механіка
-Павленко О.В
-карп 304</t>
+    <t>Компьютери та компьютерні технології
+Бєлова С. А
+гнк  324</t>
   </si>
   <si>
     <t>- пара онлайн</t>
   </si>
   <si>
-    <t>Ціноутворення
-Прогонюк
-м 203</t>
-  </si>
-  <si>
-    <t>Основиохорони праці. Охорона праці і галузі. БЖД. Основи екології
+    <t>Діловоддство 
+Марценюк А. В
+гнк 217</t>
+  </si>
+  <si>
+    <t>Аграрне право
+Гузенко Ю.І
+гнк 215</t>
+  </si>
+  <si>
+    <t>Основи охорони праці. БЖД
 Рачков О. М
-карп 111</t>
+гнк 112</t>
+  </si>
+  <si>
+    <t>Компьютери та компьютерні технології
+Бєлова С. А
+гнк 324</t>
+  </si>
+  <si>
+    <t>Паливо-мастильні та інші експлуатаційні матеріали
+Лимар О. О
+крил 013</t>
   </si>
   <si>
     <t>- асинхронно</t>
@@ -601,66 +643,71 @@
     <t>Аі 4/1</t>
   </si>
   <si>
-    <t>Організація виробничої і бізнесової діяльності
-Прогонюк Л. Ю
-м</t>
-  </si>
-  <si>
-    <t>Гнк, М, Карп</t>
-  </si>
-  <si>
-    <t>Кр</t>
-  </si>
-  <si>
-    <t>І</t>
-  </si>
-  <si>
-    <t>8.30</t>
-  </si>
-  <si>
-    <t>9.50</t>
-  </si>
-  <si>
-    <t>9.00</t>
-  </si>
-  <si>
-    <t>10.20</t>
-  </si>
-  <si>
-    <t>ІІІ</t>
-  </si>
-  <si>
-    <t>11.25</t>
-  </si>
-  <si>
-    <t>10.35</t>
-  </si>
-  <si>
-    <t>11.55</t>
-  </si>
-  <si>
-    <t>13.15</t>
-  </si>
-  <si>
-    <t>12.25</t>
-  </si>
-  <si>
-    <t>13.45</t>
-  </si>
-  <si>
-    <t>Основи бухгалтерського обліку. Економіка виробництва продукції тваринництва 
-Марковська Т. С
-гнк 102</t>
-  </si>
-  <si>
-    <t>Автоматизація технологічних процесів і системи атоматичного керування
-Садовий О. С
-крил 014</t>
+    <t>Технологія вирщування риби
+Данильчук Г. А
+карп 106</t>
   </si>
   <si>
     <t>Машини та обладнання для переробки с/г продукції
 Доценко Н. А
-крил 015</t>
+крил 006</t>
+  </si>
+  <si>
+    <t>Пк, М, Карп</t>
+  </si>
+  <si>
+    <t>Крил</t>
+  </si>
+  <si>
+    <t>І</t>
+  </si>
+  <si>
+    <t>8.30</t>
+  </si>
+  <si>
+    <t>9.50</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>10.20</t>
+  </si>
+  <si>
+    <t>Експлуатація і ремонт електрообладнання і засобів автоматизації
+Плацканов В. В
+крил 205</t>
+  </si>
+  <si>
+    <t>Експлуатація машинно-тратарного парку
+Павленко О.В
+крил 006</t>
+  </si>
+  <si>
+    <t>ІІІ</t>
+  </si>
+  <si>
+    <t>11.25</t>
+  </si>
+  <si>
+    <t>10.35</t>
+  </si>
+  <si>
+    <t>11.55</t>
+  </si>
+  <si>
+    <t>13.15</t>
+  </si>
+  <si>
+    <t>12.25</t>
+  </si>
+  <si>
+    <t>13.45</t>
+  </si>
+  <si>
+    <t>Фізичне виховання
+Рябов Є. І
+Карп с/з</t>
   </si>
   <si>
     <t>ІV</t>
@@ -690,19 +737,14 @@
     <t>16.55</t>
   </si>
   <si>
-    <t>Технології зберігання та переробки продукції рослинництва 
-Стеблічнко О. І
-гнк 118</t>
-  </si>
-  <si>
-    <t>Технологія виробництва молока і яловичини 
-Крамаренко О.С
-карп 215а</t>
-  </si>
-  <si>
-    <t>Кормовиробництво
-Кругленко А. М
-карп 110</t>
+    <t>Організація виробництва 
+Кисляк Г. М
+ГНК 303</t>
+  </si>
+  <si>
+    <t>Конярство
+Онищенко Л. В
+карп 220</t>
   </si>
 </sst>
 </file>
@@ -726,7 +768,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="16.0"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
@@ -759,6 +801,12 @@
       <name val="Times New Roman"/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -797,12 +845,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="16.0"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <sz val="15.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -826,7 +868,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,26 +889,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEAD1DC"/>
-        <bgColor rgb="FFEAD1DC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF93C47D"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -883,6 +919,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor theme="5"/>
       </patternFill>
@@ -891,12 +933,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6AA84F"/>
-        <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
     <fill>
@@ -918,7 +954,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border/>
     <border>
       <left style="thick">
@@ -1000,6 +1036,17 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thick">
         <color rgb="FF000000"/>
       </top>
@@ -1084,6 +1131,11 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1095,12 +1147,7 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
+      <right style="thick">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -1124,12 +1171,26 @@
       </bottom>
     </border>
     <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
     </border>
     <border>
-      <bottom style="thin">
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -1137,9 +1198,35 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -1148,6 +1235,20 @@
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -1159,6 +1260,36 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -1167,36 +1298,33 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thick">
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -1205,6 +1333,9 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -1216,80 +1347,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
         <color rgb="FF000000"/>
       </right>
     </border>
@@ -1297,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="109">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1305,7 +1365,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1342,236 +1402,191 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="19" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="20" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="19" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="24" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="26" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="27" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="28" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="29" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="7" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="30" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="31" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="32" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="33" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="34" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="8" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="35" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="37" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="38" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="39" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="40" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="41" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="42" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="43" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="24" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="38" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="44" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="30" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="32" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="33" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="40" fillId="8" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="34" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="36" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="25" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="37" fillId="10" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="26" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="39" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="40" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="11" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="41" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="12" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="13" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="9" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1580,37 +1595,31 @@
     <xf borderId="4" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="38" fillId="14" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="40" fillId="13" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="38" fillId="15" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="40" fillId="14" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="13" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="14" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="15" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="14" fontId="20" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="13" fontId="20" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1977,27 +1986,33 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="C4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="20"/>
       <c r="H4" s="19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I4" s="20"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="J4" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
       <c r="M4" s="21"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="N4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="22"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="23"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -2016,14 +2031,14 @@
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="29"/>
       <c r="I5" s="30"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28"/>
@@ -2049,35 +2064,33 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="33"/>
-      <c r="C6" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="35"/>
+      <c r="C6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="38" t="s">
+      <c r="F6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="40" t="s">
+      <c r="G6" s="36"/>
+      <c r="H6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="41"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="35"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="37"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -2096,20 +2109,20 @@
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="29"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="42"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="31"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -2128,36 +2141,42 @@
       <c r="A8" s="32">
         <v>3.0</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="45" t="s">
+      <c r="B8" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="35"/>
+      <c r="F8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="37"/>
-      <c r="L8" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="37"/>
-      <c r="N8" s="46" t="s">
+      <c r="I8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="37"/>
-      <c r="P8" s="45" t="s">
+      <c r="J8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="41"/>
+      <c r="K8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="38"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="35"/>
+      <c r="P8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="39"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -2174,22 +2193,22 @@
     </row>
     <row r="9" ht="72.0" customHeight="1">
       <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="30"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="29"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="30"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
       <c r="L9" s="29"/>
-      <c r="M9" s="30"/>
+      <c r="M9" s="28"/>
       <c r="N9" s="29"/>
       <c r="O9" s="30"/>
       <c r="P9" s="29"/>
-      <c r="Q9" s="42"/>
+      <c r="Q9" s="40"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -2208,41 +2227,41 @@
       <c r="A10" s="32">
         <v>4.0</v>
       </c>
-      <c r="B10" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="39" t="s">
+      <c r="B10" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="39" t="s">
+      <c r="K10" s="35"/>
+      <c r="L10" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="39" t="s">
-        <v>28</v>
-      </c>
       <c r="M10" s="35"/>
-      <c r="N10" s="40" t="s">
+      <c r="N10" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="37"/>
-      <c r="P10" s="46" t="s">
+      <c r="O10" s="35"/>
+      <c r="P10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="50"/>
+      <c r="Q10" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
@@ -2259,19 +2278,19 @@
       <c r="B11" s="26"/>
       <c r="C11" s="30"/>
       <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
       <c r="N11" s="29"/>
       <c r="O11" s="30"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="42"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="31"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -2290,36 +2309,34 @@
       <c r="A12" s="32">
         <v>5.0</v>
       </c>
-      <c r="B12" s="51" t="s">
-        <v>41</v>
+      <c r="B12" s="41" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="35"/>
-      <c r="D12" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="34" t="s">
+      <c r="D12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="46"/>
+      <c r="L12" s="34" t="s">
+        <v>30</v>
+      </c>
       <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="52" t="s">
-        <v>44</v>
-      </c>
+      <c r="N12" s="36"/>
+      <c r="O12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="39"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -2335,23 +2352,23 @@
       <c r="AD12" s="6"/>
     </row>
     <row r="13" ht="72.0" customHeight="1">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="56"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="51"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -2382,7 +2399,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="5"/>
       <c r="O14" s="6"/>
-      <c r="P14" s="50"/>
+      <c r="P14" s="45"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -2398,60 +2415,60 @@
       <c r="AD14" s="6"/>
     </row>
     <row r="15" ht="21.0" customHeight="1">
-      <c r="A15" s="57"/>
-      <c r="B15" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="58" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="C15" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="58" t="s">
+      <c r="D15" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="E15" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="58" t="s">
+      <c r="F15" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="58" t="s">
+      <c r="G15" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="58" t="s">
+      <c r="H15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="I15" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="L15" s="58" t="s">
+      <c r="J15" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="M15" s="58" t="s">
+      <c r="K15" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="N15" s="58" t="s">
+      <c r="L15" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="58" t="s">
+      <c r="M15" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="P15" s="58" t="s">
+      <c r="N15" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="Q15" s="58" t="s">
+      <c r="O15" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="R15" s="58" t="s">
+      <c r="P15" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="S15" s="59" t="s">
+      <c r="Q15" s="53" t="s">
         <v>62</v>
+      </c>
+      <c r="R15" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" s="54" t="s">
+        <v>64</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -2466,37 +2483,37 @@
       <c r="AD15" s="6"/>
     </row>
     <row r="16" ht="44.25" customHeight="1">
-      <c r="A16" s="60">
+      <c r="A16" s="55">
         <v>1.0</v>
       </c>
-      <c r="B16" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="63" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="64" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="P16" s="65" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="66"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="23"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
@@ -2511,21 +2528,21 @@
     <row r="17" ht="56.25" customHeight="1">
       <c r="A17" s="26"/>
       <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="30"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="57"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
       <c r="S17" s="31"/>
       <c r="T17" s="6"/>
@@ -2540,43 +2557,47 @@
       <c r="AC17" s="6"/>
     </row>
     <row r="18" ht="57.0" customHeight="1">
-      <c r="A18" s="67">
+      <c r="A18" s="58">
         <v>2.0</v>
       </c>
-      <c r="B18" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="35"/>
+      <c r="B18" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>71</v>
+      </c>
       <c r="D18" s="35"/>
-      <c r="E18" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="37"/>
-      <c r="K18" s="35"/>
+      <c r="E18" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="35"/>
+      <c r="K18" s="34" t="s">
+        <v>76</v>
+      </c>
       <c r="L18" s="35"/>
-      <c r="M18" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="N18" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="O18" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="P18" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="70"/>
+      <c r="M18" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="N18" s="59"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="R18" s="36"/>
+      <c r="S18" s="37"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
@@ -2591,21 +2612,21 @@
     <row r="19" ht="63.75" customHeight="1">
       <c r="A19" s="26"/>
       <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="29"/>
       <c r="F19" s="30"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="29"/>
       <c r="J19" s="30"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="30"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
       <c r="R19" s="28"/>
       <c r="S19" s="31"/>
       <c r="T19" s="6"/>
@@ -2620,47 +2641,47 @@
       <c r="AC19" s="6"/>
     </row>
     <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" s="67">
+      <c r="A20" s="58">
         <v>3.0</v>
       </c>
-      <c r="B20" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>78</v>
+      <c r="B20" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>83</v>
       </c>
       <c r="H20" s="35"/>
-      <c r="I20" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="L20" s="37"/>
-      <c r="M20" s="35"/>
+      <c r="I20" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="K20" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" s="35"/>
+      <c r="M20" s="34" t="s">
+        <v>86</v>
+      </c>
       <c r="N20" s="35"/>
-      <c r="O20" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="P20" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="69" t="s">
-        <v>83</v>
-      </c>
-      <c r="S20" s="70"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="S20" s="39"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
@@ -2675,23 +2696,23 @@
     <row r="21" ht="79.5" customHeight="1">
       <c r="A21" s="26"/>
       <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="29"/>
       <c r="J21" s="30"/>
       <c r="K21" s="29"/>
       <c r="L21" s="30"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
       <c r="Q21" s="30"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="31"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="40"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
@@ -2704,39 +2725,49 @@
       <c r="AC21" s="6"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="67">
+      <c r="A22" s="58">
         <v>4.0</v>
       </c>
-      <c r="B22" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="L22" s="37"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="46" t="s">
+      <c r="B22" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="S22" s="41"/>
+      <c r="C22" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="L22" s="35"/>
+      <c r="M22" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="O22" s="36"/>
+      <c r="P22" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R22" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="S22" s="39"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
@@ -2750,11 +2781,11 @@
     </row>
     <row r="23" ht="85.5" customHeight="1">
       <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="48"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="30"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="29"/>
       <c r="H23" s="30"/>
       <c r="I23" s="28"/>
@@ -2767,7 +2798,7 @@
       <c r="P23" s="28"/>
       <c r="Q23" s="28"/>
       <c r="R23" s="29"/>
-      <c r="S23" s="42"/>
+      <c r="S23" s="40"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
@@ -2780,41 +2811,39 @@
       <c r="AC23" s="6"/>
     </row>
     <row r="24" ht="34.5" customHeight="1">
-      <c r="A24" s="67">
+      <c r="A24" s="58">
         <v>5.0</v>
       </c>
-      <c r="B24" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="75" t="s">
+      <c r="B24" s="60"/>
+      <c r="C24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="L24" s="37"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="P24" s="35"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="34" t="s">
+        <v>100</v>
+      </c>
       <c r="Q24" s="35"/>
-      <c r="R24" s="76"/>
-      <c r="S24" s="41"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="44" t="s">
+        <v>98</v>
+      </c>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
@@ -2827,25 +2856,25 @@
       <c r="AC24" s="6"/>
     </row>
     <row r="25" ht="55.5" customHeight="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="79"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="62"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
@@ -2858,16 +2887,16 @@
       <c r="AC25" s="6"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="80"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="81"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -2887,42 +2916,42 @@
       <c r="AA26" s="6"/>
     </row>
     <row r="27" ht="19.5" customHeight="1">
-      <c r="A27" s="82"/>
-      <c r="B27" s="83" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="84" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="84" t="s">
-        <v>98</v>
-      </c>
-      <c r="E27" s="84" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="84" t="s">
+      <c r="A27" s="65"/>
+      <c r="B27" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="H27" s="84" t="s">
+      <c r="C27" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="I27" s="84" t="s">
+      <c r="D27" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="J27" s="84" t="s">
+      <c r="E27" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="K27" s="84" t="s">
+      <c r="F27" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="L27" s="84" t="s">
+      <c r="G27" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="M27" s="85" t="s">
+      <c r="H27" s="67" t="s">
         <v>107</v>
+      </c>
+      <c r="I27" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="K27" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="L27" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="M27" s="68" t="s">
+        <v>112</v>
       </c>
       <c r="N27" s="5"/>
       <c r="O27" s="6"/>
@@ -2943,27 +2972,25 @@
       <c r="A28" s="16">
         <v>1.0</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="N28" s="87"/>
-      <c r="O28" s="88" t="s">
-        <v>111</v>
+      <c r="B28" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="71" t="s">
+        <v>115</v>
       </c>
       <c r="P28" s="14"/>
       <c r="Q28" s="15"/>
@@ -2980,22 +3007,22 @@
     </row>
     <row r="29" ht="57.75" customHeight="1">
       <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="29"/>
-      <c r="J29" s="30"/>
+      <c r="J29" s="57"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="31"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="53"/>
-      <c r="P29" s="89"/>
-      <c r="Q29" s="79"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="51"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
@@ -3011,36 +3038,34 @@
       <c r="A30" s="32">
         <v>2.0</v>
       </c>
-      <c r="B30" s="90"/>
-      <c r="C30" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="75" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="44" t="s">
+      <c r="B30" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="J30" s="37"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="92" t="s">
+      <c r="C30" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="N30" s="87"/>
-      <c r="O30" s="93"/>
-      <c r="P30" s="94" t="s">
+      <c r="D30" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="Q30" s="79"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="J30" s="35"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="M30" s="37"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q30" s="51"/>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
       <c r="T30" s="6"/>
@@ -3055,21 +3080,21 @@
     <row r="31" ht="75.75" customHeight="1">
       <c r="A31" s="26"/>
       <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="29"/>
       <c r="J31" s="30"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
       <c r="M31" s="31"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="97"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="79"/>
+      <c r="Q31" s="80"/>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
       <c r="T31" s="6"/>
@@ -3085,36 +3110,36 @@
       <c r="A32" s="32">
         <v>3.0</v>
       </c>
-      <c r="B32" s="90"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="81"/>
+      <c r="E32" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="35"/>
+      <c r="G32" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="18"/>
+      <c r="I32" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="J32" s="35"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H32" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="I32" s="75"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="98" t="s">
-        <v>122</v>
-      </c>
-      <c r="M32" s="37"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="99"/>
-      <c r="P32" s="100" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q32" s="97"/>
+      <c r="M32" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="N32" s="70"/>
+      <c r="O32" s="83"/>
+      <c r="P32" s="84" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q32" s="80"/>
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
@@ -3129,21 +3154,21 @@
     <row r="33" ht="82.5" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="57"/>
       <c r="F33" s="30"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="29"/>
       <c r="J33" s="30"/>
       <c r="K33" s="28"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="78"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="97"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="78"/>
+      <c r="P33" s="79"/>
+      <c r="Q33" s="80"/>
       <c r="R33" s="6"/>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
@@ -3155,40 +3180,42 @@
       <c r="Z33" s="6"/>
       <c r="AA33" s="6"/>
     </row>
-    <row r="34" ht="52.5" customHeight="1">
+    <row r="34" ht="76.5" customHeight="1">
       <c r="A34" s="32">
         <v>4.0</v>
       </c>
-      <c r="B34" s="90"/>
-      <c r="C34" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="35"/>
       <c r="G34" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="H34" s="101" t="s">
-        <v>120</v>
-      </c>
-      <c r="I34" s="75"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="35"/>
+      <c r="I34" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="J34" s="59"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="M34" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="M34" s="102"/>
-      <c r="N34" s="87"/>
-      <c r="O34" s="103"/>
-      <c r="P34" s="100" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q34" s="97"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="88"/>
+      <c r="P34" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q34" s="80"/>
       <c r="R34" s="6"/>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
@@ -3200,24 +3227,24 @@
       <c r="Z34" s="6"/>
       <c r="AA34" s="6"/>
     </row>
-    <row r="35" ht="78.0" customHeight="1">
+    <row r="35" ht="76.5" customHeight="1">
       <c r="A35" s="26"/>
       <c r="B35" s="27"/>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="30"/>
       <c r="I35" s="29"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="28"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="30"/>
       <c r="L35" s="28"/>
       <c r="M35" s="31"/>
-      <c r="N35" s="87"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="97"/>
+      <c r="N35" s="70"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="80"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
       <c r="T35" s="6"/>
@@ -3233,32 +3260,36 @@
       <c r="A36" s="32">
         <v>5.0</v>
       </c>
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
-      <c r="I36" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="J36" s="37"/>
-      <c r="K36" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="L36" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="M36" s="102"/>
-      <c r="N36" s="87"/>
-      <c r="O36" s="104"/>
-      <c r="P36" s="100" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q36" s="97"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="36"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="35"/>
+      <c r="I36" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="J36" s="90"/>
+      <c r="K36" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M36" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="N36" s="70"/>
+      <c r="O36" s="91"/>
+      <c r="P36" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q36" s="80"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
       <c r="T36" s="6"/>
@@ -3271,25 +3302,25 @@
       <c r="AA36" s="6"/>
     </row>
     <row r="37" ht="55.5" customHeight="1">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="78"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="87"/>
-      <c r="O37" s="105" t="s">
-        <v>132</v>
-      </c>
-      <c r="P37" s="96"/>
-      <c r="Q37" s="97"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="70"/>
+      <c r="O37" s="92" t="s">
+        <v>141</v>
+      </c>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="80"/>
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
       <c r="T37" s="6"/>
@@ -3317,7 +3348,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="5"/>
       <c r="O38" s="6"/>
-      <c r="P38" s="106"/>
+      <c r="P38" s="93"/>
       <c r="S38" s="6"/>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
@@ -3329,21 +3360,21 @@
       <c r="AA38" s="6"/>
     </row>
     <row r="39" ht="24.0" customHeight="1">
-      <c r="A39" s="107"/>
-      <c r="B39" s="108" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" s="109" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="110" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="110" t="s">
-        <v>136</v>
-      </c>
-      <c r="F39" s="111" t="s">
-        <v>137</v>
+      <c r="A39" s="94"/>
+      <c r="B39" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="96" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="97" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39" s="98" t="s">
+        <v>146</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3364,33 +3395,33 @@
       <c r="Z39" s="6"/>
     </row>
     <row r="40" ht="67.5" customHeight="1">
-      <c r="A40" s="112">
+      <c r="A40" s="16">
         <v>1.0</v>
       </c>
       <c r="B40" s="17"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="113" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="98" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="37"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="99" t="s">
+        <v>148</v>
+      </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="114" t="s">
-        <v>139</v>
-      </c>
-      <c r="I40" s="96"/>
-      <c r="J40" s="97"/>
+      <c r="H40" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" s="79"/>
+      <c r="J40" s="80"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="115" t="s">
-        <v>140</v>
-      </c>
-      <c r="M40" s="96"/>
-      <c r="N40" s="97"/>
+      <c r="L40" s="101" t="s">
+        <v>150</v>
+      </c>
+      <c r="M40" s="79"/>
+      <c r="N40" s="80"/>
       <c r="O40" s="6"/>
-      <c r="P40" s="116"/>
-      <c r="Q40" s="116"/>
+      <c r="P40" s="102"/>
+      <c r="Q40" s="102"/>
       <c r="S40" s="6"/>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
@@ -3401,34 +3432,34 @@
       <c r="Z40" s="6"/>
     </row>
     <row r="41" ht="61.5" customHeight="1">
-      <c r="A41" s="29"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="27"/>
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="78"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="117" t="s">
-        <v>141</v>
-      </c>
-      <c r="I41" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="J41" s="117" t="s">
-        <v>143</v>
+      <c r="H41" s="103" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="103" t="s">
+        <v>152</v>
+      </c>
+      <c r="J41" s="103" t="s">
+        <v>153</v>
       </c>
       <c r="K41" s="3"/>
-      <c r="L41" s="118" t="s">
-        <v>141</v>
-      </c>
-      <c r="M41" s="118" t="s">
-        <v>144</v>
-      </c>
-      <c r="N41" s="118" t="s">
-        <v>145</v>
+      <c r="L41" s="104" t="s">
+        <v>151</v>
+      </c>
+      <c r="M41" s="104" t="s">
+        <v>154</v>
+      </c>
+      <c r="N41" s="104" t="s">
+        <v>155</v>
       </c>
       <c r="O41" s="6"/>
-      <c r="P41" s="116"/>
+      <c r="P41" s="102"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
@@ -3439,39 +3470,43 @@
       <c r="Z41" s="6"/>
     </row>
     <row r="42" ht="69.0" customHeight="1">
-      <c r="A42" s="112">
+      <c r="A42" s="32">
         <v>2.0</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="E42" s="75"/>
-      <c r="F42" s="41"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="44" t="s">
+        <v>157</v>
+      </c>
       <c r="G42" s="3"/>
-      <c r="H42" s="117" t="s">
-        <v>146</v>
-      </c>
-      <c r="I42" s="119">
+      <c r="H42" s="103" t="s">
+        <v>158</v>
+      </c>
+      <c r="I42" s="105">
         <v>45787.0</v>
       </c>
-      <c r="J42" s="117" t="s">
-        <v>147</v>
+      <c r="J42" s="103" t="s">
+        <v>159</v>
       </c>
       <c r="K42" s="3"/>
-      <c r="L42" s="118" t="s">
-        <v>146</v>
-      </c>
-      <c r="M42" s="118" t="s">
-        <v>148</v>
-      </c>
-      <c r="N42" s="118" t="s">
-        <v>149</v>
+      <c r="L42" s="104" t="s">
+        <v>158</v>
+      </c>
+      <c r="M42" s="104" t="s">
+        <v>160</v>
+      </c>
+      <c r="N42" s="104" t="s">
+        <v>161</v>
       </c>
       <c r="O42" s="6"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
+      <c r="P42" s="102"/>
+      <c r="Q42" s="102"/>
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
@@ -3482,34 +3517,34 @@
       <c r="Z42" s="6"/>
     </row>
     <row r="43" ht="58.5" customHeight="1">
-      <c r="A43" s="29"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="42"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="31"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="117" t="s">
-        <v>146</v>
-      </c>
-      <c r="I43" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="J43" s="117" t="s">
-        <v>150</v>
+      <c r="H43" s="103" t="s">
+        <v>158</v>
+      </c>
+      <c r="I43" s="103" t="s">
+        <v>161</v>
+      </c>
+      <c r="J43" s="103" t="s">
+        <v>162</v>
       </c>
       <c r="K43" s="3"/>
-      <c r="L43" s="118" t="s">
-        <v>146</v>
-      </c>
-      <c r="M43" s="118" t="s">
-        <v>151</v>
-      </c>
-      <c r="N43" s="118" t="s">
-        <v>152</v>
+      <c r="L43" s="104" t="s">
+        <v>158</v>
+      </c>
+      <c r="M43" s="104" t="s">
+        <v>163</v>
+      </c>
+      <c r="N43" s="104" t="s">
+        <v>164</v>
       </c>
       <c r="O43" s="6"/>
-      <c r="P43" s="116"/>
+      <c r="P43" s="102"/>
       <c r="S43" s="6"/>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
@@ -3520,43 +3555,41 @@
       <c r="Z43" s="6"/>
     </row>
     <row r="44" ht="69.0" customHeight="1">
-      <c r="A44" s="112">
+      <c r="A44" s="32">
         <v>3.0</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="69" t="s">
-        <v>154</v>
-      </c>
-      <c r="F44" s="120" t="s">
-        <v>155</v>
-      </c>
+      <c r="B44" s="60"/>
+      <c r="C44" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" s="35"/>
+      <c r="E44" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F44" s="37"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="117" t="s">
-        <v>156</v>
-      </c>
-      <c r="I44" s="117" t="s">
-        <v>157</v>
-      </c>
-      <c r="J44" s="117" t="s">
-        <v>158</v>
+      <c r="H44" s="103" t="s">
+        <v>166</v>
+      </c>
+      <c r="I44" s="103" t="s">
+        <v>167</v>
+      </c>
+      <c r="J44" s="103" t="s">
+        <v>168</v>
       </c>
       <c r="K44" s="3"/>
-      <c r="L44" s="118" t="s">
-        <v>156</v>
-      </c>
-      <c r="M44" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="N44" s="118" t="s">
-        <v>160</v>
+      <c r="L44" s="104" t="s">
+        <v>166</v>
+      </c>
+      <c r="M44" s="104" t="s">
+        <v>169</v>
+      </c>
+      <c r="N44" s="104" t="s">
+        <v>170</v>
       </c>
       <c r="O44" s="6"/>
-      <c r="P44" s="116"/>
-      <c r="Q44" s="116"/>
+      <c r="P44" s="102"/>
+      <c r="Q44" s="102"/>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
@@ -3567,34 +3600,34 @@
       <c r="Z44" s="6"/>
     </row>
     <row r="45" ht="54.0" customHeight="1">
-      <c r="A45" s="29"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="28"/>
       <c r="F45" s="31"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="117" t="s">
-        <v>161</v>
-      </c>
-      <c r="I45" s="119">
+      <c r="H45" s="103" t="s">
+        <v>171</v>
+      </c>
+      <c r="I45" s="105">
         <v>45792.0</v>
       </c>
-      <c r="J45" s="117" t="s">
-        <v>162</v>
+      <c r="J45" s="103" t="s">
+        <v>172</v>
       </c>
       <c r="K45" s="3"/>
-      <c r="L45" s="118" t="s">
-        <v>161</v>
-      </c>
-      <c r="M45" s="118" t="s">
-        <v>163</v>
-      </c>
-      <c r="N45" s="118" t="s">
-        <v>164</v>
+      <c r="L45" s="104" t="s">
+        <v>171</v>
+      </c>
+      <c r="M45" s="104" t="s">
+        <v>173</v>
+      </c>
+      <c r="N45" s="104" t="s">
+        <v>174</v>
       </c>
       <c r="O45" s="6"/>
-      <c r="P45" s="116"/>
+      <c r="P45" s="102"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
@@ -3605,24 +3638,20 @@
       <c r="Z45" s="6"/>
     </row>
     <row r="46" ht="64.5" customHeight="1">
-      <c r="A46" s="112">
+      <c r="A46" s="32">
         <v>4.0</v>
       </c>
-      <c r="B46" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="D46" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="E46" s="69" t="s">
-        <v>154</v>
-      </c>
-      <c r="F46" s="120" t="s">
-        <v>155</v>
-      </c>
+      <c r="B46" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="36"/>
+      <c r="D46" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F46" s="37"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3632,8 +3661,8 @@
       <c r="M46" s="3"/>
       <c r="N46" s="5"/>
       <c r="O46" s="6"/>
-      <c r="P46" s="116"/>
-      <c r="Q46" s="116"/>
+      <c r="P46" s="102"/>
+      <c r="Q46" s="102"/>
       <c r="S46" s="6"/>
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
@@ -3644,21 +3673,21 @@
       <c r="Z46" s="6"/>
     </row>
     <row r="47" ht="73.5" customHeight="1">
-      <c r="A47" s="29"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="27"/>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="28"/>
       <c r="F47" s="31"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="116"/>
-      <c r="I47" s="116"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="102"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="5"/>
       <c r="O47" s="6"/>
-      <c r="P47" s="121"/>
+      <c r="P47" s="106"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
@@ -3669,20 +3698,18 @@
       <c r="Z47" s="6"/>
     </row>
     <row r="48" ht="47.25" customHeight="1">
-      <c r="A48" s="112">
+      <c r="A48" s="32">
         <v>5.0</v>
       </c>
       <c r="B48" s="33"/>
-      <c r="C48" s="69" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="E48" s="35"/>
-      <c r="F48" s="70"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E48" s="36"/>
+      <c r="F48" s="37"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="116"/>
+      <c r="H48" s="102"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -3701,15 +3728,15 @@
       <c r="Z48" s="6"/>
     </row>
     <row r="49" ht="61.5" customHeight="1">
-      <c r="A49" s="29"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="56"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="62"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="116"/>
+      <c r="H49" s="102"/>
+      <c r="I49" s="102"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -3735,11 +3762,11 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="116"/>
+      <c r="H50" s="102"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="122"/>
+      <c r="N50" s="107"/>
     </row>
     <row r="51" ht="67.5" customHeight="1">
       <c r="A51" s="1"/>
@@ -3749,12 +3776,12 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="116"/>
-      <c r="I51" s="116"/>
+      <c r="H51" s="102"/>
+      <c r="I51" s="102"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="122"/>
+      <c r="N51" s="107"/>
     </row>
     <row r="52" ht="58.5" customHeight="1">
       <c r="A52" s="1"/>
@@ -3764,11 +3791,11 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="116"/>
+      <c r="H52" s="102"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="122"/>
+      <c r="N52" s="107"/>
     </row>
     <row r="53" ht="72.0" customHeight="1">
       <c r="A53" s="1"/>
@@ -3778,12 +3805,12 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="116"/>
-      <c r="I53" s="116"/>
+      <c r="H53" s="102"/>
+      <c r="I53" s="102"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="122"/>
+      <c r="N53" s="107"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1"/>
@@ -3911,19 +3938,19 @@
       <c r="M61" s="1"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="123"/>
-      <c r="B62" s="123"/>
-      <c r="C62" s="123"/>
-      <c r="D62" s="123"/>
-      <c r="E62" s="123"/>
-      <c r="F62" s="123"/>
-      <c r="G62" s="123"/>
-      <c r="H62" s="123"/>
-      <c r="I62" s="123"/>
-      <c r="J62" s="123"/>
-      <c r="K62" s="123"/>
-      <c r="L62" s="123"/>
-      <c r="M62" s="123"/>
+      <c r="A62" s="108"/>
+      <c r="B62" s="108"/>
+      <c r="C62" s="108"/>
+      <c r="D62" s="108"/>
+      <c r="E62" s="108"/>
+      <c r="F62" s="108"/>
+      <c r="G62" s="108"/>
+      <c r="H62" s="108"/>
+      <c r="I62" s="108"/>
+      <c r="J62" s="108"/>
+      <c r="K62" s="108"/>
+      <c r="L62" s="108"/>
+      <c r="M62" s="108"/>
     </row>
     <row r="63" ht="15.75" customHeight="1"/>
     <row r="64" ht="15.75" customHeight="1"/>
@@ -4863,267 +4890,258 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="260">
-    <mergeCell ref="G30:H31"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="I32:J33"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="P47:R47"/>
+  <mergeCells count="251">
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="H4:I5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="J4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="S24:S25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="I34:K35"/>
+    <mergeCell ref="I36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="O37:Q37"/>
     <mergeCell ref="P38:R39"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:H37"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="L40:N40"/>
     <mergeCell ref="Q40:R40"/>
     <mergeCell ref="P41:R41"/>
     <mergeCell ref="Q42:R42"/>
     <mergeCell ref="P43:R43"/>
     <mergeCell ref="Q44:R44"/>
     <mergeCell ref="P45:R45"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:Q25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="O28:Q29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:O9"/>
+    <mergeCell ref="P8:Q9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:K11"/>
+    <mergeCell ref="L10:M11"/>
+    <mergeCell ref="N10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="K18:L19"/>
+    <mergeCell ref="M18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D19"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="I18:J19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="K20:L21"/>
+    <mergeCell ref="M20:N21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:Q21"/>
+    <mergeCell ref="R20:S21"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G20:H21"/>
+    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="K22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
     <mergeCell ref="O22:O23"/>
     <mergeCell ref="P22:P23"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:M33"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E40:F41"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="I16:J17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="N8:O9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="P6:Q7"/>
-    <mergeCell ref="P8:Q9"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="N10:O11"/>
-    <mergeCell ref="P10:Q11"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="P16:Q17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="R24:S25"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:F43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="I34:J35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="I36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="S20:S21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:J21"/>
-    <mergeCell ref="K20:L21"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:Q21"/>
     <mergeCell ref="Q22:Q23"/>
     <mergeCell ref="R22:S23"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:Q19"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="O37:Q37"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:L25"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="O28:Q29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="G22:H23"/>
+    <mergeCell ref="I22:I23"/>
     <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:L23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="G28:H29"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="I32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
     <mergeCell ref="P32:Q32"/>
     <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="H32:H33"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>

</xml_diff>